<commit_message>
Adição da classe UtilitarioCadastroTestCase
</commit_message>
<xml_diff>
--- a/projeto-base-selenium/src/test/java/SISTEMA/transacoes/cadastro_pessoas/pessoa/PessoaTest.xlsx
+++ b/projeto-base-selenium/src/test/java/SISTEMA/transacoes/cadastro_pessoas/pessoa/PessoaTest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\ws_robo\projeto-base-selenium\src\test\java\SISTEMA\cadastro_pessoas\pessoa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felipem.medeiros\Documents\02-cursos\java\base-selenio\projeto-base-selenium\src\test\java\SISTEMA\transacoes\cadastro_pessoas\pessoa\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -74,10 +74,10 @@
     <t>33133133131</t>
   </si>
   <si>
-    <t>@TESTE</t>
-  </si>
-  <si>
     <t>pkPessoa</t>
+  </si>
+  <si>
+    <t>@TESTE - @teste</t>
   </si>
 </sst>
 </file>
@@ -454,7 +454,7 @@
   <dimension ref="B1:J2"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -472,7 +472,7 @@
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -522,7 +522,7 @@
         <v>2</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>13</v>

</xml_diff>